<commit_message>
HR added to FTP
</commit_message>
<xml_diff>
--- a/poznamky/FTP-test/ftp-test.xlsx
+++ b/poznamky/FTP-test/ftp-test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="5700" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="5200" yWindow="5700" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Power Based Training Zones" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Time</t>
   </si>
@@ -213,6 +213,12 @@
     <t>HR:  (may not be achieved during initial phases of effort(s))
 Just below to just above TT effort, taking into account duration, current fitness, environmental conditions, etc. Essentially continuous sensation of moderate or even greater leg effort/fatigue. Continuous conversation difficult at best, due to depth/frequency of breathing. Effort sufficiently high that sustained exercise at this level is mentally very taxing - therefore typically performed in training as multiple 'repeats', 'modules', or 'blocks' of 10-30 min duration. Consecutive days of training at level 4 possible, but such workouts generally only performed when sufficiently rested/recovered from prior training so as to be able to maintain intensity.</t>
   </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>bmp</t>
+  </si>
 </sst>
 </file>
 
@@ -367,7 +373,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,8 +399,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -501,8 +519,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -515,6 +543,12 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -527,6 +561,12 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -856,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -869,12 +909,14 @@
     <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49" style="6" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="55" style="6" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" style="45" customWidth="1"/>
+    <col min="8" max="8" width="49" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -886,16 +928,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="7"/>
+    <row r="2" spans="1:10" s="5" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="7">
+        <v>165</v>
+      </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="13"/>
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="13"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -911,14 +961,16 @@
       <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="105">
+    <row r="4" spans="1:10" ht="105">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -935,17 +987,24 @@
       <c r="E4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12">
+        <f>B2*0.68</f>
+        <v>112.2</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="I4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="J4" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="150">
+    <row r="5" spans="1:10" ht="150">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -963,17 +1022,25 @@
       <c r="E5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="12">
+        <f>B2*0.69</f>
+        <v>113.85</v>
+      </c>
+      <c r="G5" s="12">
+        <f>B2*0.83</f>
+        <v>136.94999999999999</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="I5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="150">
+    <row r="6" spans="1:10" ht="150">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -991,17 +1058,25 @@
       <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="12">
+        <f>B2*0.84</f>
+        <v>138.6</v>
+      </c>
+      <c r="G6" s="12">
+        <f>B2*0.94</f>
+        <v>155.1</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="I6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="J6" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="195">
+    <row r="7" spans="1:10" ht="195">
       <c r="A7" s="10">
         <v>4</v>
       </c>
@@ -1019,17 +1094,25 @@
       <c r="E7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="12">
+        <f>B2*0.95</f>
+        <v>156.75</v>
+      </c>
+      <c r="G7" s="12">
+        <f>B2*1.05</f>
+        <v>173.25</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="I7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="J7" s="19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="135">
+    <row r="8" spans="1:10" ht="135">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -1047,17 +1130,22 @@
       <c r="E8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="12">
+        <f>B2*1.06</f>
+        <v>174.9</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="I8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="J8" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="90">
+    <row r="9" spans="1:10" ht="90">
       <c r="A9" s="10">
         <v>6</v>
       </c>
@@ -1074,17 +1162,19 @@
       <c r="E9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="I9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="J9" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60">
+    <row r="10" spans="1:10" ht="60">
       <c r="A10" s="10">
         <v>7</v>
       </c>
@@ -1098,117 +1188,119 @@
         <v>32</v>
       </c>
       <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="J10" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="G13" s="22" t="s">
+    <row r="13" spans="1:10">
+      <c r="I13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="J13" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="G14" s="20">
-        <v>0</v>
-      </c>
-      <c r="H14" s="21" t="s">
+    <row r="14" spans="1:10">
+      <c r="I14" s="20">
+        <v>0</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="G15" s="20" t="s">
+    <row r="15" spans="1:10">
+      <c r="I15" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="J15" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="G16" s="20">
+    <row r="16" spans="1:10">
+      <c r="I16" s="20">
         <v>1</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="J16" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="7:8">
-      <c r="G17" s="20">
+    <row r="17" spans="9:10">
+      <c r="I17" s="20">
         <v>2</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="J17" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="7:8">
-      <c r="G18" s="20">
+    <row r="18" spans="9:10">
+      <c r="I18" s="20">
         <v>3</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="J18" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="7:8">
-      <c r="G19" s="20">
+    <row r="19" spans="9:10">
+      <c r="I19" s="20">
         <v>4</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="J19" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="7:8">
-      <c r="G20" s="20">
+    <row r="20" spans="9:10">
+      <c r="I20" s="20">
         <v>5</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="J20" s="21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="7:8">
-      <c r="G21" s="20">
+    <row r="21" spans="9:10">
+      <c r="I21" s="20">
         <v>6</v>
       </c>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="7:8">
-      <c r="G22" s="20">
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="9:10">
+      <c r="I22" s="20">
         <v>7</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="J22" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="7:8">
-      <c r="G23" s="20">
+    <row r="23" spans="9:10">
+      <c r="I23" s="20">
         <v>8</v>
       </c>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="7:8">
-      <c r="G24" s="20">
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="9:10">
+      <c r="I24" s="20">
         <v>9</v>
       </c>
-      <c r="H24" s="21"/>
-    </row>
-    <row r="25" spans="7:8">
-      <c r="G25" s="20">
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="9:10">
+      <c r="I25" s="20">
         <v>10</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="J25" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="7:8">
-      <c r="G26" s="20" t="s">
+    <row r="26" spans="9:10">
+      <c r="I26" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="J26" s="21" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1225,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1238,7 +1330,7 @@
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="25">
+    <row r="2" spans="1:5" ht="25">
       <c r="A2" s="24" t="str">
         <f>'Power Based Training Zones'!B4</f>
         <v>Active Recovery</v>
@@ -1251,8 +1343,16 @@
         <f>'Power Based Training Zones'!D4</f>
         <v>94.050000000000011</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="25">
+      <c r="D2" s="31">
+        <f>'Power Based Training Zones'!F4</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="31">
+        <f>'Power Based Training Zones'!G4</f>
+        <v>112.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25">
       <c r="A3" s="25" t="str">
         <f>'Power Based Training Zones'!B5</f>
         <v>Endurance</v>
@@ -1265,8 +1365,16 @@
         <f>'Power Based Training Zones'!D5</f>
         <v>128.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="25">
+      <c r="D3" s="32">
+        <f>'Power Based Training Zones'!F5</f>
+        <v>113.85</v>
+      </c>
+      <c r="E3" s="32">
+        <f>'Power Based Training Zones'!G5</f>
+        <v>136.94999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25">
       <c r="A4" s="26" t="str">
         <f>'Power Based Training Zones'!B6</f>
         <v>Tempo</v>
@@ -1279,8 +1387,16 @@
         <f>'Power Based Training Zones'!D6</f>
         <v>153.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="25">
+      <c r="D4" s="33">
+        <f>'Power Based Training Zones'!F6</f>
+        <v>138.6</v>
+      </c>
+      <c r="E4" s="33">
+        <f>'Power Based Training Zones'!G6</f>
+        <v>155.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="25">
       <c r="A5" s="27" t="str">
         <f>'Power Based Training Zones'!B7</f>
         <v>Lactate Threshold</v>
@@ -1293,8 +1409,16 @@
         <f>'Power Based Training Zones'!D7</f>
         <v>179.55</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="25">
+      <c r="D5" s="34">
+        <f>'Power Based Training Zones'!F7</f>
+        <v>156.75</v>
+      </c>
+      <c r="E5" s="34">
+        <f>'Power Based Training Zones'!G7</f>
+        <v>173.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="25">
       <c r="A6" s="28" t="str">
         <f>'Power Based Training Zones'!B8</f>
         <v>VO2 Max</v>
@@ -1307,8 +1431,13 @@
         <f>'Power Based Training Zones'!D8</f>
         <v>205.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="25">
+      <c r="D6" s="35">
+        <f>'Power Based Training Zones'!F8</f>
+        <v>174.9</v>
+      </c>
+      <c r="E6" s="35"/>
+    </row>
+    <row r="7" spans="1:5" ht="25">
       <c r="A7" s="29" t="str">
         <f>'Power Based Training Zones'!B9</f>
         <v>Anaerobic Capacity</v>
@@ -1321,8 +1450,10 @@
         <f>'Power Based Training Zones'!D9</f>
         <v>N/A</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="25">
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+    </row>
+    <row r="8" spans="1:5" ht="25">
       <c r="A8" s="30" t="str">
         <f>'Power Based Training Zones'!B10</f>
         <v>Neuromuscular Power</v>
@@ -1335,6 +1466,8 @@
         <f>'Power Based Training Zones'!D10</f>
         <v>N/A</v>
       </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1352,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>